<commit_message>
Before: IO-fix, new transport files
</commit_message>
<xml_diff>
--- a/data/cnf_files/restore_cnf_v5.xlsx
+++ b/data/cnf_files/restore_cnf_v5.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ruiziv/switchdrive/ACCURACY/RESTORE/data/cnf_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E265C2D1-48BA-AC4C-9474-25A4C4809C90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39ED8573-850F-3B4C-9ACA-5A4B38B7AB4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38400" yWindow="-4880" windowWidth="21600" windowHeight="37900" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38400" yWindow="-4880" windowWidth="21600" windowHeight="37900" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="country" sheetId="1" r:id="rId1"/>
@@ -20807,7 +20807,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:H315"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
@@ -28332,8 +28334,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:L325"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A260" workbookViewId="0">
-      <selection activeCell="I313" sqref="I313"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F48" sqref="F48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -39235,28 +39237,28 @@
       <c r="C313" s="2"/>
       <c r="D313" s="2"/>
       <c r="E313">
-        <v>14495</v>
+        <v>17394</v>
       </c>
       <c r="F313">
-        <v>4232</v>
+        <v>5078.3999999999996</v>
       </c>
       <c r="G313">
-        <v>20114</v>
+        <v>24136.799999999999</v>
       </c>
       <c r="H313">
-        <v>140689</v>
+        <v>168826.8</v>
       </c>
       <c r="I313">
-        <v>345709</v>
+        <v>414850.8</v>
       </c>
       <c r="J313">
-        <v>309</v>
+        <v>370.8</v>
       </c>
       <c r="K313">
-        <v>4619</v>
+        <v>5542.8</v>
       </c>
       <c r="L313">
-        <v>5704.6</v>
+        <v>6845.52</v>
       </c>
     </row>
     <row r="314" spans="1:12" x14ac:dyDescent="0.2">
@@ -40541,8 +40543,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:F35"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K8" sqref="K8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2:G31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -40551,6 +40553,7 @@
     <col min="2" max="2" width="13.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="13.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
@@ -40588,7 +40591,7 @@
         <v>46.578000000000003</v>
       </c>
       <c r="F2">
-        <v>52815.20640000001</v>
+        <v>70456.805717760028</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
@@ -40606,7 +40609,7 @@
         <v>47.585999999999999</v>
       </c>
       <c r="F3">
-        <v>54247.98720000001</v>
+        <v>72368.171124480024</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
@@ -40624,7 +40627,7 @@
         <v>47.866</v>
       </c>
       <c r="F4">
-        <v>53100.185600000012</v>
+        <v>70836.975095040034</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
@@ -40642,7 +40645,7 @@
         <v>47.238999999999997</v>
       </c>
       <c r="F5">
-        <v>52054.886400000018</v>
+        <v>69442.519829760029</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
@@ -40660,7 +40663,7 @@
         <v>46.896999999999998</v>
       </c>
       <c r="F6">
-        <v>50529.121280000007</v>
+        <v>67407.111015552015</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
@@ -40678,7 +40681,7 @@
         <v>47.881999999999998</v>
       </c>
       <c r="F7">
-        <v>50030.464000000007</v>
+        <v>66741.889737600024</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
@@ -40696,7 +40699,7 @@
         <v>48.692</v>
       </c>
       <c r="F8">
-        <v>50785.039360000017</v>
+        <v>67748.512132224045</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
@@ -40714,7 +40717,7 @@
         <v>48.612000000000002</v>
       </c>
       <c r="F9">
-        <v>51255.98720000001</v>
+        <v>68376.768324480028</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
@@ -40732,7 +40735,7 @@
         <v>49.62</v>
       </c>
       <c r="F10">
-        <v>51885.870080000015</v>
+        <v>69217.047833472039</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
@@ -40750,7 +40753,7 @@
         <v>51.213000000000001</v>
       </c>
       <c r="F11">
-        <v>52659.312640000026</v>
+        <v>70248.83954457604</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
@@ -40768,7 +40771,7 @@
         <v>52.372999999999998</v>
       </c>
       <c r="F12">
-        <v>53610.95168000002</v>
+        <v>71518.349814912042</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
@@ -40786,7 +40789,7 @@
         <v>53.749000000000002</v>
       </c>
       <c r="F13">
-        <v>54337.592320000011</v>
+        <v>72487.706594688032</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
@@ -40804,7 +40807,7 @@
         <v>54.029000000000003</v>
       </c>
       <c r="F14">
-        <v>55311.590400000016</v>
+        <v>73787.044383360044</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
@@ -40822,7 +40825,7 @@
         <v>55.122</v>
       </c>
       <c r="F15">
-        <v>55938.094080000017</v>
+        <v>74622.815955072045</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
@@ -40840,7 +40843,7 @@
         <v>56.170999999999999</v>
       </c>
       <c r="F16">
-        <v>56601.318400000011</v>
+        <v>75507.57377856005</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
@@ -40858,7 +40861,7 @@
         <v>57.33</v>
       </c>
       <c r="F17">
-        <v>57455.467520000013</v>
+        <v>76647.030058368036</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
@@ -40876,7 +40879,7 @@
         <v>57.781999999999996</v>
       </c>
       <c r="F18">
-        <v>58238.935040000011</v>
+        <v>77692.195316736033</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
@@ -40894,7 +40897,7 @@
         <v>57.432000000000002</v>
       </c>
       <c r="F19">
-        <v>59321.574400000012</v>
+        <v>79136.463288960033</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
@@ -40912,7 +40915,7 @@
         <v>58.728999999999999</v>
       </c>
       <c r="F20">
-        <v>60633.362847957142</v>
+        <v>80886.421873246058</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
@@ -40930,7 +40933,7 @@
         <v>57.494</v>
       </c>
       <c r="F21">
-        <v>62598.267575226506</v>
+        <v>83507.653902041566</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
@@ -40948,7 +40951,7 @@
         <v>59.784999999999997</v>
       </c>
       <c r="F22">
-        <v>64218.337054849675</v>
+        <v>85668.867089595849</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
@@ -40966,7 +40969,7 @@
         <v>58.598999999999997</v>
       </c>
       <c r="F23">
-        <v>64905.647429659788</v>
+        <v>86585.756312351936</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
@@ -40984,7 +40987,7 @@
         <v>58.972999999999999</v>
       </c>
       <c r="F24">
-        <v>65647.683092869396</v>
+        <v>87575.650437965116</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
@@ -41002,7 +41005,7 @@
         <v>59.323</v>
       </c>
       <c r="F25">
-        <v>66479.311910059114</v>
+        <v>88685.064070816632</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
@@ -41020,7 +41023,7 @@
         <v>57.466000000000001</v>
       </c>
       <c r="F26">
-        <v>67520.912622653137</v>
+        <v>90074.585461434879</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
@@ -41038,7 +41041,7 @@
         <v>58.246000000000002</v>
       </c>
       <c r="F27">
-        <v>68503.558312291192</v>
+        <v>91385.459377554289</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
@@ -41056,7 +41059,7 @@
         <v>58.238999999999997</v>
       </c>
       <c r="F28">
-        <v>69948.984946545606</v>
+        <v>93313.694643315539</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.2">
@@ -41074,7 +41077,7 @@
         <v>58.482999999999997</v>
       </c>
       <c r="F29">
-        <v>71036.37970605561</v>
+        <v>94764.306437370877</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.2">
@@ -41092,7 +41095,7 @@
         <v>57.646999999999998</v>
       </c>
       <c r="F30">
-        <v>71608.228986909948</v>
+        <v>95527.167674262557</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.2">
@@ -41110,7 +41113,7 @@
         <v>57.198</v>
       </c>
       <c r="F31">
-        <v>72950.000564662536</v>
+        <v>97317.124503273968</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
IO-fixes: flexible DataHanlder - added get() and get_fxe(), lenient reads - Empty annual variables no longer trigger errors - capacity_to_activity is now annual - new generic input/output_share constraints - Passenger sector has not short and long travel demands
</commit_message>
<xml_diff>
--- a/data/cnf_files/restore_cnf_v5.xlsx
+++ b/data/cnf_files/restore_cnf_v5.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10312"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10409"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ruiziv/switchdrive/ACCURACY/RESTORE/data/cnf_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39ED8573-850F-3B4C-9ACA-5A4B38B7AB4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39C3C65D-F98C-BC46-9587-9B2FDC1DD97E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38400" yWindow="-4880" windowWidth="21600" windowHeight="37900" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38400" yWindow="-4880" windowWidth="21600" windowHeight="37900" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="country" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4407" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4409" uniqueCount="114">
   <si>
     <t>Type</t>
   </si>
@@ -376,10 +376,13 @@
     <t>enable_max_import_share</t>
   </si>
   <si>
-    <t>flow_in_max_share</t>
+    <t>max_share_at_in_flow</t>
   </si>
   <si>
-    <t>flow_out_max_share</t>
+    <t>max_share_at_out_flow</t>
+  </si>
+  <si>
+    <t>annual_fxe</t>
   </si>
 </sst>
 </file>
@@ -3896,9 +3899,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:I321"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A258" workbookViewId="0">
+      <selection activeCell="A312" sqref="A312"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="12.1640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
@@ -9633,12 +9647,14 @@
     </row>
     <row r="310" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A310" s="2" t="s">
-        <v>5</v>
+        <v>113</v>
       </c>
       <c r="B310" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="C310" s="2"/>
+      <c r="C310" s="2" t="s">
+        <v>54</v>
+      </c>
       <c r="D310" s="2"/>
       <c r="G310">
         <v>0.4</v>
@@ -9646,12 +9662,14 @@
     </row>
     <row r="311" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A311" s="2" t="s">
-        <v>5</v>
+        <v>113</v>
       </c>
       <c r="B311" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="C311" s="2"/>
+      <c r="C311" s="2" t="s">
+        <v>54</v>
+      </c>
       <c r="D311" s="2"/>
       <c r="G311">
         <v>0.4</v>
@@ -20807,11 +20825,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:H315"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+    <sheetView topLeftCell="A268" workbookViewId="0">
+      <selection activeCell="E309" sqref="E309"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.83203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.1640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.1640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
@@ -40543,7 +40571,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:F35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G2" sqref="G2:G31"/>
     </sheetView>
   </sheetViews>

</xml_diff>